<commit_message>
correzione colonne ID 152 e 164
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111#ESCINFORMATICASRLXX/ESC-INFORMATICA_SRL/MEDIXIS/1.0.0/report-checklist.xlsx
+++ b/GATEWAY/A1#111#ESCINFORMATICASRLXX/ESC-INFORMATICA_SRL/MEDIXIS/1.0.0/report-checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\escsrv12\Sviluppo$\MediXis\FSE2_2024\Files_Accreditamento\A1#111#ESCINFORMATICASRLXX\ESC-INFORMATICA_SRL\MEDIXIS\1.0.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7FD1529-46A0-4262-BF71-7E542AC92047}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E4EA15E-9DF5-4705-889F-931CE846388B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="483" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="484" uniqueCount="238">
   <si>
     <t>COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -993,6 +993,9 @@
   </si>
   <si>
     <t>subject_application_id: MEDIXIS</t>
+  </si>
+  <si>
+    <t>[ERRORE-6| L'elemento ClinicalDocument/confidentialityCode DEVE avere l'attributo @code valorizzato con 'N' o 'V', e il @codeSystem='2.16.840.1.113883.5.25'],[ERRORE-44| Il codice fiscale 'mdcttn62r10a944d' cittadino ed operatore deve essere costituito da 16 cifre [A-Z0-9]{16}]</t>
   </si>
 </sst>
 </file>
@@ -1510,9 +1513,6 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1549,6 +1549,9 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1571,7 +1574,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2066,7 +2069,7 @@
       <pane xSplit="1" ySplit="9" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="P12" sqref="P12"/>
+      <selection pane="bottomRight" activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15"/>
@@ -2413,7 +2416,7 @@
       <c r="M11" s="33" t="s">
         <v>60</v>
       </c>
-      <c r="N11" s="68" t="s">
+      <c r="N11" s="55" t="s">
         <v>178</v>
       </c>
       <c r="O11" s="40" t="s">
@@ -2731,7 +2734,9 @@
       <c r="M18" s="33" t="s">
         <v>60</v>
       </c>
-      <c r="N18" s="43"/>
+      <c r="N18" s="68" t="s">
+        <v>237</v>
+      </c>
       <c r="O18" s="33" t="s">
         <v>60</v>
       </c>
@@ -2781,13 +2786,13 @@
         <v>60</v>
       </c>
       <c r="K19" s="33"/>
-      <c r="L19" s="44" t="s">
+      <c r="L19" s="43" t="s">
         <v>60</v>
       </c>
-      <c r="M19" s="44" t="s">
+      <c r="M19" s="43" t="s">
         <v>60</v>
       </c>
-      <c r="N19" s="45" t="s">
+      <c r="N19" s="44" t="s">
         <v>200</v>
       </c>
       <c r="O19" s="33" t="s">
@@ -2837,13 +2842,13 @@
         <v>60</v>
       </c>
       <c r="K20" s="33"/>
-      <c r="L20" s="46" t="s">
+      <c r="L20" s="45" t="s">
         <v>60</v>
       </c>
-      <c r="M20" s="47" t="s">
+      <c r="M20" s="46" t="s">
         <v>60</v>
       </c>
-      <c r="N20" s="48" t="s">
+      <c r="N20" s="47" t="s">
         <v>199</v>
       </c>
       <c r="O20" s="25" t="s">
@@ -2968,7 +2973,7 @@
       <c r="D23" s="21" t="s">
         <v>82</v>
       </c>
-      <c r="E23" s="49" t="s">
+      <c r="E23" s="48" t="s">
         <v>83</v>
       </c>
       <c r="F23" s="23"/>
@@ -3145,7 +3150,7 @@
       <c r="M27" s="33" t="s">
         <v>60</v>
       </c>
-      <c r="N27" s="50" t="s">
+      <c r="N27" s="49" t="s">
         <v>211</v>
       </c>
       <c r="O27" s="33" t="s">
@@ -3201,7 +3206,7 @@
       <c r="M28" s="33" t="s">
         <v>60</v>
       </c>
-      <c r="N28" s="51" t="s">
+      <c r="N28" s="50" t="s">
         <v>216</v>
       </c>
       <c r="O28" s="33" t="s">
@@ -3257,7 +3262,7 @@
       <c r="M29" s="33" t="s">
         <v>60</v>
       </c>
-      <c r="N29" s="51" t="s">
+      <c r="N29" s="50" t="s">
         <v>221</v>
       </c>
       <c r="O29" s="33" t="s">
@@ -3291,9 +3296,7 @@
       <c r="E30" s="22" t="s">
         <v>97</v>
       </c>
-      <c r="F30" s="23">
-        <v>45349</v>
-      </c>
+      <c r="F30" s="23"/>
       <c r="G30" s="24"/>
       <c r="H30" s="24"/>
       <c r="I30" s="24"/>
@@ -3331,7 +3334,7 @@
       <c r="E31" s="22" t="s">
         <v>99</v>
       </c>
-      <c r="F31" s="52"/>
+      <c r="F31" s="51"/>
       <c r="G31" s="24"/>
       <c r="H31" s="24"/>
       <c r="I31" s="24"/>
@@ -3505,7 +3508,7 @@
       <c r="M35" s="33" t="s">
         <v>60</v>
       </c>
-      <c r="N35" s="50" t="s">
+      <c r="N35" s="49" t="s">
         <v>227</v>
       </c>
       <c r="O35" s="33" t="s">
@@ -3524,7 +3527,7 @@
       </c>
     </row>
     <row r="36" spans="1:20" ht="140.1" customHeight="1" thickBot="1">
-      <c r="A36" s="53">
+      <c r="A36" s="52">
         <v>374</v>
       </c>
       <c r="B36" s="37" t="s">
@@ -3536,10 +3539,10 @@
       <c r="D36" s="37" t="s">
         <v>108</v>
       </c>
-      <c r="E36" s="49" t="s">
+      <c r="E36" s="48" t="s">
         <v>109</v>
       </c>
-      <c r="F36" s="52">
+      <c r="F36" s="51">
         <v>45345</v>
       </c>
       <c r="G36" s="34" t="s">
@@ -3561,9 +3564,9 @@
       <c r="O36" s="33"/>
       <c r="P36" s="33"/>
       <c r="Q36" s="33"/>
-      <c r="R36" s="54"/>
+      <c r="R36" s="53"/>
       <c r="S36" s="41"/>
-      <c r="T36" s="55" t="s">
+      <c r="T36" s="54" t="s">
         <v>46</v>
       </c>
     </row>

</xml_diff>

<commit_message>
id 147 e 374 correzione titolo sezione Prestazioni
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111#ESCINFORMATICASRLXX/ESC-INFORMATICA_SRL/MEDIXIS/1.0.0/report-checklist.xlsx
+++ b/GATEWAY/A1#111#ESCINFORMATICASRLXX/ESC-INFORMATICA_SRL/MEDIXIS/1.0.0/report-checklist.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\escsrv12\Sviluppo$\MediXis\FSE2_2024\Files_Accreditamento\A1#111#ESCINFORMATICASRLXX\ESC-INFORMATICA_SRL\MEDIXIS\1.0.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E4EA15E-9DF5-4705-889F-931CE846388B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F937964-394B-476F-AE90-8694214B157C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Istruzioni Compilazione" sheetId="1" r:id="rId1"/>
@@ -776,21 +776,6 @@
     <t>NO</t>
   </si>
   <si>
-    <t>f630e7927c255a14</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.80.3.1.4.4.b4353945207f34564bccb5d6e6198785db3cd57f7c1f1b55f419d5637b16abb6.2f7bc3b5df^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2024-02-23T17:38:05Z</t>
-  </si>
-  <si>
-    <t>f62ad1b350b43413</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.80.3.1.4.4.a652078f79e44e1a9f271cbd3e41b3e27eed0f4b98d306d343699ca0c46b8859.3fd77b068e^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>Sezioni opzionali non gestite</t>
   </si>
   <si>
@@ -980,9 +965,6 @@
     <t>2.16.840.1.113883.2.9.2.80.3.1.4.4.7ce50f6d3b63af01daf5b37f26dd48ee2065b132dedd95203ea817eee6105709.07487cf581^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
-    <t>2024-02-23T13:40:50Z</t>
-  </si>
-  <si>
     <t>subject_application_version:1.0.0</t>
   </si>
   <si>
@@ -996,6 +978,24 @@
   </si>
   <si>
     <t>[ERRORE-6| L'elemento ClinicalDocument/confidentialityCode DEVE avere l'attributo @code valorizzato con 'N' o 'V', e il @codeSystem='2.16.840.1.113883.5.25'],[ERRORE-44| Il codice fiscale 'mdcttn62r10a944d' cittadino ed operatore deve essere costituito da 16 cifre [A-Z0-9]{16}]</t>
+  </si>
+  <si>
+    <t>2024-03-07T16:45Z</t>
+  </si>
+  <si>
+    <t>3c41ecce86da87f6</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.80.3.1.4.4.a652078f79e44e1a9f271cbd3e41b3e27eed0f4b98d306d343699ca0c46b8859.9f60a313ea^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2024-03-07T16:51Z</t>
+  </si>
+  <si>
+    <t>627ceffd98d556bb</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.80.3.1.4.4.b4353945207f34564bccb5d6e6198785db3cd57f7c1f1b55f419d5637b16abb6.9be3a61541^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
 </sst>
 </file>
@@ -1552,6 +1552,9 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1573,9 +1576,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2069,7 +2069,7 @@
       <pane xSplit="1" ySplit="9" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="F30" sqref="F30"/>
+      <selection pane="bottomRight" activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15"/>
@@ -2107,14 +2107,14 @@
       <c r="T1" s="15"/>
     </row>
     <row r="2" spans="1:20" ht="18.75">
-      <c r="A2" s="58" t="s">
+      <c r="A2" s="59" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="59"/>
-      <c r="C2" s="60" t="s">
-        <v>234</v>
-      </c>
-      <c r="D2" s="59"/>
+      <c r="B2" s="60"/>
+      <c r="C2" s="61" t="s">
+        <v>228</v>
+      </c>
+      <c r="D2" s="60"/>
       <c r="F2" s="12"/>
       <c r="G2" s="12"/>
       <c r="H2" s="12"/>
@@ -2132,14 +2132,14 @@
       <c r="T2" s="15"/>
     </row>
     <row r="3" spans="1:20" ht="15.75">
-      <c r="A3" s="61" t="s">
+      <c r="A3" s="62" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="62"/>
-      <c r="C3" s="67" t="s">
-        <v>236</v>
-      </c>
-      <c r="D3" s="59"/>
+      <c r="B3" s="63"/>
+      <c r="C3" s="68" t="s">
+        <v>230</v>
+      </c>
+      <c r="D3" s="60"/>
       <c r="F3" s="12"/>
       <c r="G3" s="12"/>
       <c r="H3" s="12"/>
@@ -2157,12 +2157,12 @@
       <c r="T3" s="15"/>
     </row>
     <row r="4" spans="1:20" ht="15.75">
-      <c r="A4" s="63"/>
-      <c r="B4" s="64"/>
-      <c r="C4" s="67" t="s">
-        <v>235</v>
-      </c>
-      <c r="D4" s="59"/>
+      <c r="A4" s="64"/>
+      <c r="B4" s="65"/>
+      <c r="C4" s="68" t="s">
+        <v>229</v>
+      </c>
+      <c r="D4" s="60"/>
       <c r="E4" s="4"/>
       <c r="F4" s="12"/>
       <c r="G4" s="12"/>
@@ -2181,12 +2181,12 @@
       <c r="T4" s="15"/>
     </row>
     <row r="5" spans="1:20" ht="15.75">
-      <c r="A5" s="65"/>
-      <c r="B5" s="66"/>
-      <c r="C5" s="67" t="s">
-        <v>233</v>
-      </c>
-      <c r="D5" s="59"/>
+      <c r="A5" s="66"/>
+      <c r="B5" s="67"/>
+      <c r="C5" s="68" t="s">
+        <v>227</v>
+      </c>
+      <c r="D5" s="60"/>
       <c r="F5" s="12"/>
       <c r="G5" s="12"/>
       <c r="H5" s="12"/>
@@ -2204,8 +2204,8 @@
       <c r="T5" s="15"/>
     </row>
     <row r="6" spans="1:20">
-      <c r="A6" s="56"/>
-      <c r="B6" s="57"/>
+      <c r="A6" s="57"/>
+      <c r="B6" s="58"/>
       <c r="C6" s="16"/>
       <c r="F6" s="12"/>
       <c r="G6" s="12"/>
@@ -2342,13 +2342,13 @@
         <v>45345</v>
       </c>
       <c r="G10" s="34" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="H10" s="34" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="I10" s="34" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="J10" s="25" t="s">
         <v>60</v>
@@ -2361,16 +2361,16 @@
         <v>60</v>
       </c>
       <c r="N10" s="25" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="O10" s="39" t="s">
         <v>60</v>
       </c>
       <c r="P10" s="39" t="s">
+        <v>172</v>
+      </c>
+      <c r="Q10" s="33" t="s">
         <v>177</v>
-      </c>
-      <c r="Q10" s="33" t="s">
-        <v>182</v>
       </c>
       <c r="R10" s="26"/>
       <c r="S10" s="27"/>
@@ -2398,13 +2398,13 @@
         <v>45345</v>
       </c>
       <c r="G11" s="34" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="H11" s="34" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="I11" s="34" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="J11" s="33" t="s">
         <v>60</v>
@@ -2417,16 +2417,16 @@
         <v>60</v>
       </c>
       <c r="N11" s="55" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="O11" s="40" t="s">
         <v>60</v>
       </c>
       <c r="P11" s="40" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="Q11" s="33" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="R11" s="26"/>
       <c r="S11" s="27"/>
@@ -2471,7 +2471,7 @@
         <v>60</v>
       </c>
       <c r="P12" s="40" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="Q12" s="25"/>
       <c r="R12" s="26" t="s">
@@ -2499,16 +2499,16 @@
         <v>63</v>
       </c>
       <c r="F13" s="23">
-        <v>45345</v>
+        <v>45358</v>
       </c>
       <c r="G13" s="34" t="s">
-        <v>166</v>
+        <v>232</v>
       </c>
       <c r="H13" s="34" t="s">
-        <v>167</v>
+        <v>233</v>
       </c>
       <c r="I13" s="34" t="s">
-        <v>168</v>
+        <v>234</v>
       </c>
       <c r="J13" s="25" t="s">
         <v>60</v>
@@ -2550,7 +2550,7 @@
         <v>163</v>
       </c>
       <c r="K14" s="25" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="L14" s="25"/>
       <c r="M14" s="25"/>
@@ -2588,7 +2588,7 @@
         <v>163</v>
       </c>
       <c r="K15" s="25" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="L15" s="25"/>
       <c r="M15" s="25"/>
@@ -2626,7 +2626,7 @@
         <v>163</v>
       </c>
       <c r="K16" s="25" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="L16" s="25"/>
       <c r="M16" s="25"/>
@@ -2660,13 +2660,13 @@
         <v>45345</v>
       </c>
       <c r="G17" s="34" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="H17" s="34" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="I17" s="34" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="J17" s="25" t="s">
         <v>60</v>
@@ -2679,16 +2679,16 @@
         <v>60</v>
       </c>
       <c r="N17" s="33" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="O17" s="33" t="s">
         <v>60</v>
       </c>
       <c r="P17" s="40" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="Q17" s="33" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="R17" s="26"/>
       <c r="S17" s="35"/>
@@ -2716,13 +2716,13 @@
         <v>45349</v>
       </c>
       <c r="G18" s="34" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="H18" s="34" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="I18" s="34" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="J18" s="33" t="s">
         <v>60</v>
@@ -2734,21 +2734,21 @@
       <c r="M18" s="33" t="s">
         <v>60</v>
       </c>
-      <c r="N18" s="68" t="s">
-        <v>237</v>
+      <c r="N18" s="56" t="s">
+        <v>231</v>
       </c>
       <c r="O18" s="33" t="s">
         <v>60</v>
       </c>
       <c r="P18" s="40" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="Q18" s="33" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="R18" s="26"/>
       <c r="S18" s="35" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="T18" s="28" t="s">
         <v>52</v>
@@ -2774,13 +2774,13 @@
         <v>45349</v>
       </c>
       <c r="G19" s="34" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="H19" s="34" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="I19" s="34" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="J19" s="33" t="s">
         <v>60</v>
@@ -2793,16 +2793,16 @@
         <v>60</v>
       </c>
       <c r="N19" s="44" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="O19" s="33" t="s">
         <v>60</v>
       </c>
       <c r="P19" s="39" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="Q19" s="33" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="R19" s="26"/>
       <c r="S19" s="27"/>
@@ -2830,13 +2830,13 @@
         <v>45349</v>
       </c>
       <c r="G20" s="34" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="H20" s="34" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="I20" s="34" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="J20" s="33" t="s">
         <v>60</v>
@@ -2849,16 +2849,16 @@
         <v>60</v>
       </c>
       <c r="N20" s="47" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="O20" s="25" t="s">
         <v>60</v>
       </c>
       <c r="P20" s="39" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="Q20" s="33" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="R20" s="26"/>
       <c r="S20" s="27"/>
@@ -2890,7 +2890,7 @@
         <v>163</v>
       </c>
       <c r="K21" s="33" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="L21" s="25"/>
       <c r="M21" s="25"/>
@@ -2924,13 +2924,13 @@
         <v>45349</v>
       </c>
       <c r="G22" s="34" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="H22" s="34" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="I22" s="34" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="J22" s="33" t="s">
         <v>60</v>
@@ -2943,16 +2943,16 @@
         <v>60</v>
       </c>
       <c r="N22" s="36" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="O22" s="33" t="s">
         <v>60</v>
       </c>
       <c r="P22" s="40" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="Q22" s="33" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="R22" s="26"/>
       <c r="S22" s="27"/>
@@ -2984,7 +2984,7 @@
         <v>163</v>
       </c>
       <c r="K23" s="33" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="L23" s="25"/>
       <c r="M23" s="25"/>
@@ -3022,7 +3022,7 @@
         <v>163</v>
       </c>
       <c r="K24" s="33" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="L24" s="25"/>
       <c r="M24" s="25"/>
@@ -3060,7 +3060,7 @@
         <v>163</v>
       </c>
       <c r="K25" s="33" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="L25" s="25"/>
       <c r="M25" s="25"/>
@@ -3098,7 +3098,7 @@
         <v>163</v>
       </c>
       <c r="K26" s="33" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="L26" s="25"/>
       <c r="M26" s="25"/>
@@ -3132,13 +3132,13 @@
         <v>45349</v>
       </c>
       <c r="G27" s="34" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="H27" s="34" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="I27" s="34" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="J27" s="33" t="s">
         <v>60</v>
@@ -3151,16 +3151,16 @@
         <v>60</v>
       </c>
       <c r="N27" s="49" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="O27" s="33" t="s">
         <v>60</v>
       </c>
       <c r="P27" s="40" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="Q27" s="33" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="R27" s="26"/>
       <c r="S27" s="27"/>
@@ -3188,13 +3188,13 @@
         <v>45349</v>
       </c>
       <c r="G28" s="34" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="H28" s="34" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="I28" s="34" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="J28" s="33" t="s">
         <v>60</v>
@@ -3207,16 +3207,16 @@
         <v>60</v>
       </c>
       <c r="N28" s="50" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="O28" s="33" t="s">
         <v>60</v>
       </c>
       <c r="P28" s="40" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="Q28" s="33" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="R28" s="26"/>
       <c r="S28" s="27"/>
@@ -3244,13 +3244,13 @@
         <v>45349</v>
       </c>
       <c r="G29" s="34" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="H29" s="34" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="I29" s="34" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="J29" s="33" t="s">
         <v>60</v>
@@ -3263,16 +3263,16 @@
         <v>60</v>
       </c>
       <c r="N29" s="50" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="O29" s="33" t="s">
         <v>60</v>
       </c>
       <c r="P29" s="33" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="Q29" s="33" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="R29" s="26"/>
       <c r="S29" s="27"/>
@@ -3304,7 +3304,7 @@
         <v>163</v>
       </c>
       <c r="K30" s="33" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="L30" s="25"/>
       <c r="M30" s="25"/>
@@ -3342,7 +3342,7 @@
         <v>163</v>
       </c>
       <c r="K31" s="33" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="L31" s="25"/>
       <c r="M31" s="25"/>
@@ -3380,7 +3380,7 @@
         <v>163</v>
       </c>
       <c r="K32" s="33" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="L32" s="25"/>
       <c r="M32" s="25"/>
@@ -3418,7 +3418,7 @@
         <v>163</v>
       </c>
       <c r="K33" s="33" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="L33" s="25"/>
       <c r="M33" s="25"/>
@@ -3456,7 +3456,7 @@
         <v>163</v>
       </c>
       <c r="K34" s="33" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="L34" s="25"/>
       <c r="M34" s="25"/>
@@ -3490,13 +3490,13 @@
         <v>45349</v>
       </c>
       <c r="G35" s="34" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="H35" s="34" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="I35" s="34" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="J35" s="33" t="s">
         <v>60</v>
@@ -3509,16 +3509,16 @@
         <v>60</v>
       </c>
       <c r="N35" s="49" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="O35" s="33" t="s">
         <v>60</v>
       </c>
       <c r="P35" s="40" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="Q35" s="33" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="R35" s="26"/>
       <c r="S35" s="27"/>
@@ -3543,16 +3543,16 @@
         <v>109</v>
       </c>
       <c r="F36" s="51">
-        <v>45345</v>
+        <v>45358</v>
       </c>
       <c r="G36" s="34" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="H36" s="34" t="s">
-        <v>164</v>
+        <v>236</v>
       </c>
       <c r="I36" s="34" t="s">
-        <v>165</v>
+        <v>237</v>
       </c>
       <c r="J36" s="33" t="s">
         <v>60</v>

</xml_diff>